<commit_message>
Refatora estrutura de arquivos de Report Frontend e Backend
</commit_message>
<xml_diff>
--- a/docs/reports/Test_Execution_Report-API.xlsx
+++ b/docs/reports/Test_Execution_Report-API.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="56">
   <si>
     <t>Test Case</t>
   </si>
@@ -40,7 +40,7 @@
     <t>Wesley C.</t>
   </si>
   <si>
-    <t>Failed</t>
+    <t>Passed</t>
   </si>
   <si>
     <t>BC-258 RESERVATIONS - [Admin] Cancelar/Excluir uma reserva</t>
@@ -79,9 +79,6 @@
     <t>Filmes</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>BC-231 USERS - [Common User] Tentar listar usuários</t>
   </si>
   <si>
@@ -167,6 +164,21 @@
   </si>
   <si>
     <t>BC-235 MOVIES - [Público] Listar todos os filmes</t>
+  </si>
+  <si>
+    <t>BC-267 API INFO - Obter Informações da API</t>
+  </si>
+  <si>
+    <t>API Info</t>
+  </si>
+  <si>
+    <t>BC-269 SETUP - [Dev] Criar Usuários de Teste Padrão</t>
+  </si>
+  <si>
+    <t>Setup</t>
+  </si>
+  <si>
+    <t>BC-268 SETUP - [Dev] Criar Usuário Administrador</t>
   </si>
 </sst>
 </file>
@@ -327,10 +339,10 @@
         <color rgb="FF284E3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -338,13 +350,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -352,13 +364,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </left>
       <right style="thin">
         <color rgb="FF284E3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF6F8F9"/>
       </top>
       <bottom style="thin">
         <color rgb="FF284E3F"/>
@@ -368,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -391,7 +403,7 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -403,13 +415,31 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -475,7 +505,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E38" displayName="Tabela_1" name="Tabela_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:E41" displayName="Tabela_1" name="Tabela_1" id="1">
   <tableColumns count="5">
     <tableColumn name="Test Case" id="1"/>
     <tableColumn name="Test Cycle" id="2"/>
@@ -898,47 +928,47 @@
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>22</v>
+      <c r="E12" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>22</v>
+      <c r="E13" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>22</v>
+      <c r="E14" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>21</v>
@@ -949,13 +979,13 @@
       <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>22</v>
+      <c r="E15" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>21</v>
@@ -966,33 +996,33 @@
       <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>22</v>
+      <c r="E16" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="C17" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>22</v>
+      <c r="E17" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>7</v>
@@ -1000,16 +1030,16 @@
       <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>22</v>
+      <c r="E18" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>7</v>
@@ -1017,16 +1047,16 @@
       <c r="D19" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>22</v>
+      <c r="E19" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>7</v>
@@ -1034,16 +1064,16 @@
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>22</v>
+      <c r="E20" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>7</v>
@@ -1051,16 +1081,16 @@
       <c r="D21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>22</v>
+      <c r="E21" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>7</v>
@@ -1068,16 +1098,16 @@
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>22</v>
+      <c r="E22" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>7</v>
@@ -1085,16 +1115,16 @@
       <c r="D23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>22</v>
+      <c r="E23" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>7</v>
@@ -1102,16 +1132,16 @@
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>22</v>
+      <c r="E24" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>7</v>
@@ -1119,13 +1149,13 @@
       <c r="D25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>22</v>
+      <c r="E25" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>21</v>
@@ -1136,13 +1166,13 @@
       <c r="D26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>22</v>
+      <c r="E26" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>21</v>
@@ -1153,16 +1183,16 @@
       <c r="D27" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>22</v>
+      <c r="E27" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>7</v>
@@ -1170,13 +1200,13 @@
       <c r="D28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>22</v>
+      <c r="E28" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>16</v>
@@ -1187,13 +1217,13 @@
       <c r="D29" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>22</v>
+      <c r="E29" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>16</v>
@@ -1204,16 +1234,16 @@
       <c r="D30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>22</v>
+      <c r="E30" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>7</v>
@@ -1221,16 +1251,16 @@
       <c r="D31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>22</v>
+      <c r="E31" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>7</v>
@@ -1238,16 +1268,16 @@
       <c r="D32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>22</v>
+      <c r="E32" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>7</v>
@@ -1255,13 +1285,13 @@
       <c r="D33" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="11" t="s">
-        <v>22</v>
+      <c r="E33" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>16</v>
@@ -1272,16 +1302,16 @@
       <c r="D34" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>22</v>
+      <c r="E34" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>7</v>
@@ -1289,16 +1319,16 @@
       <c r="D35" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="11" t="s">
-        <v>22</v>
+      <c r="E35" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>7</v>
@@ -1306,13 +1336,13 @@
       <c r="D36" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>22</v>
+      <c r="E36" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>21</v>
@@ -1323,30 +1353,78 @@
       <c r="D37" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="11" t="s">
-        <v>22</v>
+      <c r="E37" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
+      <c r="B39" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="42" ht="15.75" customHeight="1"/>
     <row r="43" ht="15.75" customHeight="1"/>
     <row r="44" ht="15.75" customHeight="1"/>
@@ -2308,10 +2386,10 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="B2:B38">
-      <formula1>"Reservas,Sessões,Filmes,Usuários,Salas,Autenticação"</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="B2:B41">
+      <formula1>"Reservas,Sessões,Filmes,Usuários,Salas,Autenticação,API Info,Setup"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E38">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E41">
       <formula1>"Failed,Passed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>